<commit_message>
Pie Chart & Yearly chart
</commit_message>
<xml_diff>
--- a/input/Dash_LCOE_ConfigurationV4.xlsx
+++ b/input/Dash_LCOE_ConfigurationV4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\LCOEcalc\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808EF4CC-7581-4DE4-A5AB-258F8BB3C7CA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053222D3-5C44-45B6-8738-5461EE688802}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16770" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="54">
   <si>
     <t>component</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>cost_CO2_per_tonne</t>
+  </si>
+  <si>
+    <t>CO2_costIncrease_percent_per_year</t>
   </si>
 </sst>
 </file>
@@ -622,17 +625,17 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="81.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="35.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="81.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="35.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -653,7 +656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>0</v>
       </c>
@@ -676,7 +679,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -699,7 +702,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -722,7 +725,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -745,7 +748,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -768,7 +771,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -791,7 +794,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -814,7 +817,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -837,7 +840,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -860,7 +863,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -883,7 +886,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -906,7 +909,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -929,7 +932,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -952,7 +955,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -975,7 +978,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -1021,7 +1024,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>18</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1136,7 +1139,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>21</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -1205,7 +1208,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>24</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -1251,7 +1254,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>30</v>
       </c>
@@ -1366,7 +1369,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -1389,7 +1392,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -1412,7 +1415,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>33</v>
       </c>
@@ -1435,7 +1438,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>36</v>
       </c>
@@ -1499,22 +1502,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5708E7F0-2DE7-4611-91D4-02BADD085AA2}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="64.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -1538,7 +1541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1564,7 +1567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1616,7 +1619,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1642,7 +1645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1668,7 +1671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1694,7 +1697,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1720,7 +1723,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1746,7 +1749,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1772,7 +1775,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1815,16 +1818,16 @@
         <v>44</v>
       </c>
       <c r="F12" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G12" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H12" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1841,311 +1844,368 @@
         <v>45</v>
       </c>
       <c r="F13" s="5">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="G13" s="5">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="H13" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="5">
+        <v>10</v>
+      </c>
+      <c r="G14" s="5">
+        <v>10</v>
+      </c>
+      <c r="H14" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="5">
+        <v>5</v>
+      </c>
+      <c r="G15" s="5">
+        <v>5</v>
+      </c>
+      <c r="H15" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="5">
+        <v>20</v>
+      </c>
+      <c r="G16" s="5">
+        <v>20</v>
+      </c>
+      <c r="H16" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -2161,25 +2221,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA1301B-A377-4F3E-A07F-0E5926CDAB2B}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="72.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="72.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="30.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="1"/>
     <col min="9" max="9" width="19" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -2206,7 +2266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -2235,7 +2295,7 @@
         <v>9.3709256844850056E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2264,7 +2324,7 @@
         <v>6.51890482398957E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -2293,7 +2353,7 @@
         <v>0.12222946544980444</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -2310,19 +2370,19 @@
         <v>43</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
+        <v>-10</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-10</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-10</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -2339,19 +2399,19 @@
         <v>44</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
+        <v>-25</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-25</v>
+      </c>
+      <c r="H6" s="1">
+        <v>-25</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -2368,19 +2428,19 @@
         <v>45</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
+        <v>-5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>-5</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -2399,7 +2459,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
@@ -2416,7 +2476,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
@@ -2433,7 +2493,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
@@ -2445,7 +2505,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
@@ -2457,7 +2517,7 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2465,7 +2525,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2473,7 +2533,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2481,7 +2541,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2489,7 +2549,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2497,7 +2557,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2505,7 +2565,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2513,7 +2573,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2521,7 +2581,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2529,7 +2589,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2537,7 +2597,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2545,7 +2605,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2553,7 +2613,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2561,7 +2621,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2569,7 +2629,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2577,7 +2637,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2585,7 +2645,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2593,7 +2653,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2601,7 +2661,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2609,7 +2669,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2617,7 +2677,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2625,7 +2685,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2633,7 +2693,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2641,7 +2701,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2649,7 +2709,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2657,7 +2717,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2665,7 +2725,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2673,7 +2733,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2681,7 +2741,7 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -2689,7 +2749,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -2697,7 +2757,7 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -2705,7 +2765,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -2713,7 +2773,7 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -2721,7 +2781,7 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -2729,7 +2789,7 @@
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -2737,7 +2797,7 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -2745,7 +2805,7 @@
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -2753,7 +2813,7 @@
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -2761,7 +2821,7 @@
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -2769,7 +2829,7 @@
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -2777,7 +2837,7 @@
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -2785,7 +2845,7 @@
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -2793,7 +2853,7 @@
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2810,22 +2870,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16DF341-8C1A-4D19-88F8-FE2D2A0FBA8F}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="90.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="35.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="90.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="35.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="45.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -2846,7 +2906,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -2869,7 +2929,7 @@
         <v>9.4971605452992547E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2893,7 +2953,7 @@
         <v>8.5474444907693292E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -2917,7 +2977,7 @@
         <v>1.044687659982918E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -2934,13 +2994,13 @@
         <v>43</v>
       </c>
       <c r="F5" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -2957,13 +3017,13 @@
         <v>44</v>
       </c>
       <c r="F6" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -2980,13 +3040,13 @@
         <v>45</v>
       </c>
       <c r="F7" s="5">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -2997,7 +3057,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -3012,7 +3072,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -3027,7 +3087,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
@@ -3040,7 +3100,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
@@ -3053,7 +3113,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3062,7 +3122,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -3071,7 +3131,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -3080,7 +3140,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -3089,7 +3149,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -3098,7 +3158,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -3107,7 +3167,7 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -3116,7 +3176,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -3125,7 +3185,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3134,7 +3194,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -3143,7 +3203,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -3152,7 +3212,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -3161,7 +3221,7 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -3170,7 +3230,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -3179,7 +3239,7 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -3188,7 +3248,7 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -3197,7 +3257,7 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -3206,7 +3266,7 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -3215,7 +3275,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -3224,7 +3284,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -3233,7 +3293,7 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -3242,7 +3302,7 @@
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -3251,7 +3311,7 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -3260,7 +3320,7 @@
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -3269,7 +3329,7 @@
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -3278,7 +3338,7 @@
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -3287,7 +3347,7 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -3296,7 +3356,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -3305,7 +3365,7 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -3314,7 +3374,7 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -3323,7 +3383,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -3332,7 +3392,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -3341,7 +3401,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -3350,7 +3410,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -3359,7 +3419,7 @@
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -3368,7 +3428,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -3377,7 +3437,7 @@
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -3386,7 +3446,7 @@
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -3395,7 +3455,7 @@
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -3404,7 +3464,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -3413,7 +3473,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -3422,7 +3482,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -3431,7 +3491,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -3440,19 +3500,19 @@
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
     </row>
@@ -3469,12 +3529,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>35</v>
       </c>
@@ -3486,7 +3546,7 @@
       </c>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>44855</v>
       </c>
@@ -3497,7 +3557,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>44887</v>
       </c>
@@ -3508,7 +3568,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>44889</v>
       </c>
@@ -3519,7 +3579,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>44905</v>
       </c>
@@ -3530,7 +3590,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>45063</v>
       </c>
@@ -3541,12 +3601,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>

</xml_diff>